<commit_message>
posting from excel data
</commit_message>
<xml_diff>
--- a/src/main/resources/routes/hacknu-dev-data.xlsx
+++ b/src/main/resources/routes/hacknu-dev-data.xlsx
@@ -1,26 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paradox/Downloads/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F7C33B5-7150-DB48-9A49-ABE02AEA7F74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="dev1" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="dev2" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="dev3" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="dev4" sheetId="4" r:id="rId7"/>
-    <sheet state="visible" name="dev5" sheetId="5" r:id="rId8"/>
-    <sheet state="visible" name="dev6" sheetId="6" r:id="rId9"/>
-    <sheet state="visible" name="dev7" sheetId="7" r:id="rId10"/>
-    <sheet state="visible" name="dev8" sheetId="8" r:id="rId11"/>
-    <sheet state="visible" name="dev9" sheetId="9" r:id="rId12"/>
-    <sheet state="visible" name="dev10" sheetId="10" r:id="rId13"/>
+    <sheet name="dev1" sheetId="1" r:id="rId1"/>
+    <sheet name="dev2" sheetId="2" r:id="rId2"/>
+    <sheet name="dev3" sheetId="3" r:id="rId3"/>
+    <sheet name="dev4" sheetId="4" r:id="rId4"/>
+    <sheet name="dev5" sheetId="5" r:id="rId5"/>
+    <sheet name="dev6" sheetId="6" r:id="rId6"/>
+    <sheet name="dev7" sheetId="7" r:id="rId7"/>
+    <sheet name="dev8" sheetId="8" r:id="rId8"/>
+    <sheet name="dev9" sheetId="9" r:id="rId9"/>
+    <sheet name="dev10" sheetId="10" r:id="rId10"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="21">
   <si>
     <t>Latitude</t>
   </si>
@@ -76,9 +85,6 @@
     <t>cycling</t>
   </si>
   <si>
-    <t>two people 6ps</t>
-  </si>
-  <si>
     <t>Charlie</t>
   </si>
   <si>
@@ -91,36 +97,40 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000000"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color rgb="FFEA4335"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
@@ -130,94 +140,57 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="10">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="1" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -407,28 +380,31 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="21.63"/>
-    <col customWidth="1" min="2" max="2" width="19.88"/>
-    <col customWidth="1" min="4" max="4" width="9.63"/>
-    <col customWidth="1" min="7" max="7" width="16.5"/>
-    <col customWidth="1" min="8" max="8" width="14.38"/>
-    <col customWidth="1" min="9" max="9" width="27.0"/>
+    <col min="1" max="1" width="21.6640625" customWidth="1"/>
+    <col min="2" max="2" width="19.83203125" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" customWidth="1"/>
+    <col min="7" max="7" width="16.5" customWidth="1"/>
+    <col min="8" max="8" width="14.33203125" customWidth="1"/>
+    <col min="9" max="9" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -462,57 +438,58 @@
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
     </row>
-    <row r="2">
+    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2">
-        <v>35.6609342754636</v>
+        <v>35.660934275463603</v>
       </c>
       <c r="B2" s="2">
         <v>139.729033427753</v>
       </c>
       <c r="C2" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E2" s="2">
-        <v>4875.0</v>
+        <v>4875</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>10</v>
       </c>
       <c r="G2" s="2">
-        <v>2.314</v>
+        <v>2.3140000000000001</v>
       </c>
       <c r="H2" s="2">
-        <v>0.612</v>
+        <v>0.61199999999999999</v>
       </c>
       <c r="I2" s="2">
-        <v>0.6827</v>
+        <v>0.68269999999999997</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="3"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -544,190 +521,191 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2">
-        <v>27.9744586954417</v>
+        <v>27.974458695441701</v>
       </c>
       <c r="B2" s="2">
-        <v>86.9327615931465</v>
+        <v>86.932761593146495</v>
       </c>
       <c r="C2" s="2">
-        <v>7904.99498543182</v>
+        <v>7904.9949854318202</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E2" s="2">
-        <v>93429.0</v>
+        <v>93429</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>10</v>
       </c>
       <c r="G2" s="2">
-        <v>100.21873</v>
+        <v>100.21872999999999</v>
       </c>
       <c r="H2" s="2">
         <v>100.23782</v>
       </c>
       <c r="I2" s="2">
-        <v>0.6827</v>
+        <v>0.68269999999999997</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2">
         <v>27.9782944118062</v>
       </c>
       <c r="B3" s="2">
-        <v>86.9328289345355</v>
+        <v>86.932828934535493</v>
       </c>
       <c r="C3" s="2">
-        <v>8030.23562859161</v>
+        <v>8030.2356285916103</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E3" s="2">
-        <v>202575.0</v>
+        <v>202575</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>10</v>
       </c>
       <c r="G3" s="2">
-        <v>120.23892</v>
+        <v>120.23891999999999</v>
       </c>
       <c r="H3" s="2">
-        <v>90.12783</v>
+        <v>90.127830000000003</v>
       </c>
       <c r="I3" s="2">
-        <v>0.6827</v>
+        <v>0.68269999999999997</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2">
-        <v>27.9822500528831</v>
+        <v>27.982250052883099</v>
       </c>
       <c r="B4" s="2">
-        <v>86.9292212536339</v>
+        <v>86.929221253633898</v>
       </c>
       <c r="C4" s="2">
-        <v>8418.22895971594</v>
+        <v>8418.2289597159397</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E4" s="2">
-        <v>284259.0</v>
+        <v>284259</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>10</v>
       </c>
       <c r="G4" s="2">
-        <v>95.71283</v>
+        <v>95.712829999999997</v>
       </c>
       <c r="H4" s="2">
-        <v>85.23982</v>
+        <v>85.239819999999995</v>
       </c>
       <c r="I4" s="2">
-        <v>0.6827</v>
+        <v>0.68269999999999997</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2">
-        <v>27.986113230619</v>
+        <v>27.986113230619001</v>
       </c>
       <c r="B5" s="2">
-        <v>86.9268117577216</v>
+        <v>86.926811757721595</v>
       </c>
       <c r="C5" s="2">
-        <v>8667.76702937572</v>
+        <v>8667.7670293757201</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E5" s="2">
-        <v>736935.0</v>
+        <v>736935</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="G5" s="2">
-        <v>92.23824</v>
+        <v>92.238240000000005</v>
       </c>
       <c r="H5" s="2">
-        <v>60.23234</v>
+        <v>60.232340000000001</v>
       </c>
       <c r="I5" s="2">
-        <v>0.6827</v>
+        <v>0.68269999999999997</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2">
-        <v>27.9883405300116</v>
+        <v>27.988340530011602</v>
       </c>
       <c r="B6" s="2">
-        <v>86.9248104014861</v>
+        <v>86.924810401486098</v>
       </c>
       <c r="C6" s="2">
-        <v>8812.0491622451</v>
+        <v>8812.0491622451009</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E6" s="2">
-        <v>1211279.0</v>
+        <v>1211279</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>10</v>
       </c>
       <c r="G6" s="2">
-        <v>65.123823</v>
+        <v>65.123823000000002</v>
       </c>
       <c r="H6" s="2">
-        <v>40.47834</v>
+        <v>40.478340000000003</v>
       </c>
       <c r="I6" s="2">
-        <v>0.6827</v>
+        <v>0.68269999999999997</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="21.63"/>
-    <col customWidth="1" min="2" max="2" width="19.88"/>
-    <col customWidth="1" min="4" max="4" width="9.63"/>
-    <col customWidth="1" min="7" max="7" width="16.5"/>
-    <col customWidth="1" min="8" max="8" width="14.38"/>
-    <col customWidth="1" min="9" max="9" width="27.0"/>
+    <col min="1" max="1" width="21.6640625" customWidth="1"/>
+    <col min="2" max="2" width="19.83203125" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" customWidth="1"/>
+    <col min="7" max="7" width="16.5" customWidth="1"/>
+    <col min="8" max="8" width="14.33203125" customWidth="1"/>
+    <col min="9" max="9" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -761,21 +739,21 @@
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
     </row>
-    <row r="2">
+    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2">
-        <v>40.7435228393862</v>
+        <v>40.743522839386202</v>
       </c>
       <c r="B2" s="2">
-        <v>-74.006950753951</v>
+        <v>-74.006950753951003</v>
       </c>
       <c r="C2" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E2" s="2">
-        <v>2744.0</v>
+        <v>2744</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>10</v>
@@ -784,43 +762,44 @@
         <v>1.4456</v>
       </c>
       <c r="H2" s="2">
-        <v>0.26547</v>
+        <v>0.26546999999999998</v>
       </c>
       <c r="I2" s="2">
-        <v>0.6827</v>
+        <v>0.68269999999999997</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="3"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="21.63"/>
-    <col customWidth="1" min="2" max="2" width="19.88"/>
-    <col customWidth="1" min="3" max="3" width="15.0"/>
-    <col customWidth="1" min="4" max="4" width="9.63"/>
-    <col customWidth="1" min="7" max="7" width="16.5"/>
-    <col customWidth="1" min="8" max="8" width="14.38"/>
-    <col customWidth="1" min="9" max="9" width="27.0"/>
+    <col min="1" max="1" width="21.6640625" customWidth="1"/>
+    <col min="2" max="2" width="19.83203125" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" customWidth="1"/>
+    <col min="7" max="7" width="16.5" customWidth="1"/>
+    <col min="8" max="8" width="14.33203125" customWidth="1"/>
+    <col min="9" max="9" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -854,24 +833,24 @@
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
     </row>
-    <row r="2">
+    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2">
-        <v>51.5045214578877</v>
+        <v>51.504521457887698</v>
       </c>
       <c r="B2" s="2">
-        <v>-0.086503248026198</v>
+        <v>-8.6503248026198007E-2</v>
       </c>
       <c r="C2" s="2">
-        <v>60.6348371873548</v>
+        <v>60.634837187354798</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E2" s="2">
-        <v>3266.0</v>
+        <v>3266</v>
       </c>
       <c r="F2" s="2">
-        <v>19.0</v>
+        <v>19</v>
       </c>
       <c r="G2" s="2">
         <v>8.1</v>
@@ -880,40 +859,41 @@
         <v>8.9</v>
       </c>
       <c r="I2" s="2">
-        <v>0.6827</v>
+        <v>0.68269999999999997</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="3"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="21.63"/>
-    <col customWidth="1" min="2" max="2" width="19.88"/>
-    <col customWidth="1" min="3" max="3" width="16.88"/>
-    <col customWidth="1" min="4" max="4" width="9.63"/>
-    <col customWidth="1" min="7" max="7" width="16.5"/>
-    <col customWidth="1" min="8" max="8" width="14.38"/>
-    <col customWidth="1" min="9" max="9" width="27.0"/>
+    <col min="1" max="1" width="21.6640625" customWidth="1"/>
+    <col min="2" max="2" width="19.83203125" customWidth="1"/>
+    <col min="3" max="3" width="16.83203125" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" customWidth="1"/>
+    <col min="7" max="7" width="16.5" customWidth="1"/>
+    <col min="8" max="8" width="14.33203125" customWidth="1"/>
+    <col min="9" max="9" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -947,24 +927,24 @@
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
     </row>
-    <row r="2">
+    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2">
-        <v>40.7484892471959</v>
+        <v>40.748489247195899</v>
       </c>
       <c r="B2" s="2">
-        <v>-73.9855785714668</v>
+        <v>-73.985578571466803</v>
       </c>
       <c r="C2" s="2">
-        <v>89.3808279687458</v>
+        <v>89.380827968745805</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E2" s="2">
-        <v>21545.0</v>
+        <v>21545</v>
       </c>
       <c r="F2" s="2">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="G2" s="2">
         <v>8.67</v>
@@ -973,40 +953,41 @@
         <v>14.6</v>
       </c>
       <c r="I2" s="2">
-        <v>0.6827</v>
+        <v>0.68269999999999997</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="3"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="19.88"/>
-    <col customWidth="1" min="2" max="2" width="21.63"/>
-    <col customWidth="1" min="3" max="3" width="21.5"/>
-    <col customWidth="1" min="4" max="4" width="9.63"/>
-    <col customWidth="1" min="7" max="7" width="16.5"/>
-    <col customWidth="1" min="8" max="8" width="14.38"/>
-    <col customWidth="1" min="9" max="9" width="27.0"/>
+    <col min="1" max="1" width="19.83203125" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" customWidth="1"/>
+    <col min="3" max="3" width="21.5" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" customWidth="1"/>
+    <col min="7" max="7" width="16.5" customWidth="1"/>
+    <col min="8" max="8" width="14.33203125" customWidth="1"/>
+    <col min="9" max="9" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1040,53 +1021,53 @@
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
     </row>
-    <row r="2">
+    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="4">
-        <v>51.5084307498856</v>
+        <v>51.508430749885598</v>
       </c>
       <c r="B2" s="4">
-        <v>-0.0985850860961545</v>
+        <v>-9.8585086096154503E-2</v>
       </c>
       <c r="C2" s="5">
-        <v>0.65811756308103</v>
+        <v>0.65811756308102998</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E2" s="2">
-        <v>210541.0</v>
+        <v>210541</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>10</v>
       </c>
       <c r="G2" s="2">
-        <v>2.3764</v>
+        <v>2.3763999999999998</v>
       </c>
       <c r="H2" s="2">
-        <v>5.484818</v>
+        <v>5.4848179999999997</v>
       </c>
       <c r="I2" s="2">
-        <v>0.6827</v>
+        <v>0.68269999999999997</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="4">
-        <v>51.5081722295039</v>
+        <v>51.508172229503899</v>
       </c>
       <c r="B3" s="4">
-        <v>-0.0985978698818246</v>
+        <v>-9.8597869881824604E-2</v>
       </c>
       <c r="C3" s="5">
-        <v>0.18460057895524</v>
+        <v>0.18460057895524001</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E3" s="2">
-        <v>271786.0</v>
+        <v>271786</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>10</v>
@@ -1095,392 +1076,393 @@
         <v>2.8573</v>
       </c>
       <c r="H3" s="2">
-        <v>5.18274</v>
+        <v>5.1827399999999999</v>
       </c>
       <c r="I3" s="2">
-        <v>0.6827</v>
+        <v>0.68269999999999997</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="4">
-        <v>51.5084026106553</v>
+        <v>51.508402610655303</v>
       </c>
       <c r="B4" s="4">
-        <v>-0.098512050934636</v>
+        <v>-9.8512050934635997E-2</v>
       </c>
       <c r="C4" s="5">
-        <v>1.11890095321305</v>
+        <v>1.1189009532130501</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E4" s="2">
-        <v>346999.0</v>
+        <v>346999</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>10</v>
       </c>
       <c r="G4" s="2">
-        <v>2.9853</v>
+        <v>2.9853000000000001</v>
       </c>
       <c r="H4" s="2">
-        <v>5.4228294</v>
+        <v>5.4228294000000004</v>
       </c>
       <c r="I4" s="2">
-        <v>0.6827</v>
+        <v>0.68269999999999997</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="4">
-        <v>51.5086787981714</v>
+        <v>51.508678798171402</v>
       </c>
       <c r="B5" s="4">
-        <v>-0.0984920497122077</v>
+        <v>-9.8492049712207694E-2</v>
       </c>
       <c r="C5" s="5">
-        <v>6.84008048192768</v>
+        <v>6.8400804819276804</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E5" s="2">
-        <v>412323.0</v>
+        <v>412323</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="G5" s="2">
-        <v>2.55035</v>
+        <v>2.5503499999999999</v>
       </c>
       <c r="H5" s="2">
         <v>2.325053</v>
       </c>
       <c r="I5" s="2">
-        <v>0.6827</v>
+        <v>0.68269999999999997</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="4">
-        <v>51.5091735759613</v>
+        <v>51.509173575961299</v>
       </c>
       <c r="B6" s="4">
-        <v>-0.0984679986576197</v>
+        <v>-9.8467998657619696E-2</v>
       </c>
       <c r="C6" s="5">
-        <v>6.8198559137089</v>
+        <v>6.8198559137089001</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E6" s="2">
-        <v>496645.0</v>
+        <v>496645</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>10</v>
       </c>
       <c r="G6" s="2">
-        <v>2.98437</v>
+        <v>2.9843700000000002</v>
       </c>
       <c r="H6" s="2">
         <v>5.13931</v>
       </c>
       <c r="I6" s="2">
-        <v>0.6827</v>
+        <v>0.68269999999999997</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="4">
-        <v>51.5095937834761</v>
+        <v>51.509593783476099</v>
       </c>
       <c r="B7" s="4">
-        <v>-0.0984240991632801</v>
+        <v>-9.8424099163280099E-2</v>
       </c>
       <c r="C7" s="5">
-        <v>6.81997951790538</v>
+        <v>6.8199795179053799</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E7" s="2">
-        <v>556118.0</v>
+        <v>556118</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>10</v>
       </c>
       <c r="G7" s="2">
-        <v>3.292342</v>
+        <v>3.2923420000000001</v>
       </c>
       <c r="H7" s="2">
         <v>5.420242</v>
       </c>
       <c r="I7" s="2">
-        <v>0.6827</v>
+        <v>0.68269999999999997</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="6">
         <v>51.510087671925</v>
       </c>
       <c r="B8" s="6">
-        <v>-0.0983794103700441</v>
+        <v>-9.8379410370044107E-2</v>
       </c>
       <c r="C8" s="5">
-        <v>7.17710718071825</v>
+        <v>7.1771071807182496</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E8" s="2">
-        <v>616721.0</v>
+        <v>616721</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>10</v>
       </c>
       <c r="G8" s="2">
-        <v>2.45881</v>
+        <v>2.4588100000000002</v>
       </c>
       <c r="H8" s="2">
-        <v>4.92494</v>
+        <v>4.9249400000000003</v>
       </c>
       <c r="I8" s="2">
-        <v>0.6827</v>
+        <v>0.68269999999999997</v>
       </c>
       <c r="J8" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="4">
         <v>51.51052554748</v>
       </c>
       <c r="B9" s="4">
-        <v>-0.0983531343389532</v>
+        <v>-9.8353134338953194E-2</v>
       </c>
       <c r="C9" s="5">
-        <v>7.1412686889752</v>
+        <v>7.1412686889751997</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E9" s="2">
-        <v>691282.0</v>
+        <v>691282</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>10</v>
       </c>
       <c r="G9" s="2">
-        <v>2.443</v>
+        <v>2.4430000000000001</v>
       </c>
       <c r="H9" s="2">
-        <v>3.450505</v>
+        <v>3.4505050000000002</v>
       </c>
       <c r="I9" s="2">
-        <v>0.6827</v>
+        <v>0.68269999999999997</v>
       </c>
       <c r="J9" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="4">
-        <v>51.5108549650061</v>
+        <v>51.510854965006097</v>
       </c>
       <c r="B10" s="4">
-        <v>-0.0984162651626019</v>
+        <v>-9.8416265162601907E-2</v>
       </c>
       <c r="C10" s="5">
-        <v>0.20171483400944</v>
+        <v>0.20171483400944001</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E10" s="2">
-        <v>765795.0</v>
+        <v>765795</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>10</v>
       </c>
       <c r="G10" s="2">
-        <v>2.91781</v>
+        <v>2.9178099999999998</v>
       </c>
       <c r="H10" s="2">
-        <v>4.30202</v>
+        <v>4.3020199999999997</v>
       </c>
       <c r="I10" s="2">
-        <v>0.6827</v>
+        <v>0.68269999999999997</v>
       </c>
       <c r="J10" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="4">
-        <v>51.5111606123825</v>
+        <v>51.511160612382497</v>
       </c>
       <c r="B11" s="4">
-        <v>-0.0983944360105759</v>
+        <v>-9.8394436010575903E-2</v>
       </c>
       <c r="C11" s="5">
-        <v>0.2341160768048</v>
+        <v>0.23411607680480001</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E11" s="2">
-        <v>834246.0</v>
+        <v>834246</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>10</v>
       </c>
       <c r="G11" s="2">
-        <v>3.928974</v>
+        <v>3.9289740000000002</v>
       </c>
       <c r="H11" s="2">
-        <v>3.204045</v>
+        <v>3.2040449999999998</v>
       </c>
       <c r="I11" s="2">
-        <v>0.6827</v>
+        <v>0.68269999999999997</v>
       </c>
       <c r="J11" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
     </row>
-    <row r="13">
+    <row r="13" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
     </row>
-    <row r="14">
+    <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
     </row>
-    <row r="15">
+    <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
     </row>
-    <row r="16">
+    <row r="16" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
     </row>
-    <row r="17">
+    <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="4"/>
       <c r="B17" s="3"/>
       <c r="C17" s="4"/>
     </row>
-    <row r="18">
+    <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
     </row>
-    <row r="19">
+    <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="4"/>
       <c r="B19" s="5"/>
       <c r="C19" s="4"/>
     </row>
-    <row r="20">
+    <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
     </row>
-    <row r="21">
+    <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
     </row>
-    <row r="22">
+    <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
     </row>
-    <row r="23">
+    <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
     </row>
-    <row r="24">
+    <row r="24" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
     </row>
-    <row r="25">
+    <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
     </row>
-    <row r="26">
+    <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
     </row>
-    <row r="27">
+    <row r="27" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
     </row>
-    <row r="28">
+    <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
     </row>
-    <row r="29">
+    <row r="29" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
     </row>
-    <row r="30">
+    <row r="30" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
     </row>
-    <row r="33">
+    <row r="33" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B33" s="3"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:J41"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="19.13"/>
-    <col customWidth="1" min="2" max="2" width="18.5"/>
-    <col customWidth="1" min="7" max="7" width="16.5"/>
-    <col customWidth="1" min="8" max="8" width="18.13"/>
-    <col customWidth="1" min="9" max="9" width="26.63"/>
+    <col min="1" max="1" width="19.1640625" customWidth="1"/>
+    <col min="2" max="2" width="18.5" customWidth="1"/>
+    <col min="7" max="7" width="16.5" customWidth="1"/>
+    <col min="8" max="8" width="18.1640625" customWidth="1"/>
+    <col min="9" max="9" width="26.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1512,12 +1494,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="4">
         <v>40.78017131152</v>
       </c>
       <c r="B2" s="4">
-        <v>-73.9681065889423</v>
+        <v>-73.968106588942305</v>
       </c>
       <c r="C2" s="5">
         <v>1.1916338022335</v>
@@ -1526,62 +1508,62 @@
         <v>14</v>
       </c>
       <c r="E2" s="2">
-        <v>30781.0</v>
+        <v>30781</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>10</v>
       </c>
       <c r="G2" s="2">
-        <v>2.4949</v>
+        <v>2.4948999999999999</v>
       </c>
       <c r="H2" s="2">
-        <v>4.50591</v>
+        <v>4.5059100000000001</v>
       </c>
       <c r="I2" s="2">
-        <v>0.6827</v>
+        <v>0.68269999999999997</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="4">
-        <v>40.7803052985404</v>
+        <v>40.780305298540398</v>
       </c>
       <c r="B3" s="4">
-        <v>-73.9677503127735</v>
+        <v>-73.967750312773504</v>
       </c>
       <c r="C3" s="5">
-        <v>0.9427296518318</v>
+        <v>0.94272965183180002</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E3" s="2">
-        <v>60837.0</v>
+        <v>60837</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>10</v>
       </c>
       <c r="G3" s="2">
-        <v>6.9182</v>
+        <v>6.9181999999999997</v>
       </c>
       <c r="H3" s="2">
-        <v>4.40041</v>
+        <v>4.4004099999999999</v>
       </c>
       <c r="I3" s="2">
-        <v>0.6827</v>
+        <v>0.68269999999999997</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="4">
-        <v>40.7799997926053</v>
+        <v>40.779999792605302</v>
       </c>
       <c r="B4" s="4">
-        <v>-73.9670909557784</v>
+        <v>-73.967090955778403</v>
       </c>
       <c r="C4" s="5">
         <v>1.0665903523675</v>
@@ -1590,39 +1572,39 @@
         <v>14</v>
       </c>
       <c r="E4" s="2">
-        <v>91456.0</v>
+        <v>91456</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>10</v>
       </c>
       <c r="G4" s="2">
-        <v>3.0201</v>
+        <v>3.0200999999999998</v>
       </c>
       <c r="H4" s="2">
-        <v>4.29191</v>
+        <v>4.2919099999999997</v>
       </c>
       <c r="I4" s="2">
-        <v>0.6827</v>
+        <v>0.68269999999999997</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="4">
-        <v>40.7802570585996</v>
+        <v>40.780257058599602</v>
       </c>
       <c r="B5" s="4">
         <v>-73.9660506353584</v>
       </c>
       <c r="C5" s="5">
-        <v>2.5825253777544</v>
+        <v>2.5825253777544002</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E5" s="2">
-        <v>130981.0</v>
+        <v>130981</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>10</v>
@@ -1631,30 +1613,30 @@
         <v>3.95858</v>
       </c>
       <c r="H5" s="2">
-        <v>2.394499</v>
+        <v>2.3944990000000002</v>
       </c>
       <c r="I5" s="2">
-        <v>0.6827</v>
+        <v>0.68269999999999997</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="4">
-        <v>40.7811879526255</v>
+        <v>40.781187952625501</v>
       </c>
       <c r="B6" s="4">
-        <v>-73.9651698768434</v>
+        <v>-73.965169876843404</v>
       </c>
       <c r="C6" s="5">
-        <v>1.0618746729065</v>
+        <v>1.0618746729065001</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E6" s="2">
-        <v>160873.0</v>
+        <v>160873</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>10</v>
@@ -1663,21 +1645,21 @@
         <v>3.49491</v>
       </c>
       <c r="H6" s="2">
-        <v>2.344949</v>
+        <v>2.3449490000000002</v>
       </c>
       <c r="I6" s="2">
-        <v>0.6827</v>
+        <v>0.68269999999999997</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="4">
         <v>40.7820568169615</v>
       </c>
       <c r="B7" s="4">
-        <v>-73.9651399558564</v>
+        <v>-73.965139955856401</v>
       </c>
       <c r="C7" s="5">
         <v>1.3366409457624</v>
@@ -1686,7 +1668,7 @@
         <v>14</v>
       </c>
       <c r="E7" s="2">
-        <v>193475.0</v>
+        <v>193475</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>10</v>
@@ -1698,18 +1680,18 @@
         <v>2.891</v>
       </c>
       <c r="I7" s="2">
-        <v>0.6827</v>
+        <v>0.68269999999999997</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="4">
         <v>40.7825889223028</v>
       </c>
       <c r="B8" s="4">
-        <v>-73.9657080709057</v>
+        <v>-73.965708070905706</v>
       </c>
       <c r="C8" s="5">
         <v>0.3372182680177</v>
@@ -1718,39 +1700,39 @@
         <v>14</v>
       </c>
       <c r="E8" s="2">
-        <v>217847.0</v>
+        <v>217847</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>10</v>
       </c>
       <c r="G8" s="2">
-        <v>3.49872</v>
+        <v>3.4987200000000001</v>
       </c>
       <c r="H8" s="2">
-        <v>2.018911</v>
+        <v>2.0189110000000001</v>
       </c>
       <c r="I8" s="2">
-        <v>0.6827</v>
+        <v>0.68269999999999997</v>
       </c>
       <c r="J8" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="4">
-        <v>40.782394529748</v>
+        <v>40.782394529747997</v>
       </c>
       <c r="B9" s="4">
-        <v>-73.9670961006856</v>
+        <v>-73.967096100685595</v>
       </c>
       <c r="C9" s="5">
-        <v>0.7190069601966</v>
+        <v>0.71900696019660004</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E9" s="2">
-        <v>246891.0</v>
+        <v>246891</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>10</v>
@@ -1759,170 +1741,171 @@
         <v>3.58629</v>
       </c>
       <c r="H9" s="2">
-        <v>2.9891</v>
+        <v>2.9891000000000001</v>
       </c>
       <c r="I9" s="2">
-        <v>0.6827</v>
+        <v>0.68269999999999997</v>
       </c>
       <c r="J9" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="4">
-        <v>40.7816348557382</v>
+        <v>40.781634855738197</v>
       </c>
       <c r="B10" s="4">
-        <v>-73.9677941891041</v>
+        <v>-73.967794189104097</v>
       </c>
       <c r="C10" s="5">
-        <v>2.4826165065857</v>
+        <v>2.4826165065857002</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E10" s="2">
-        <v>278198.0</v>
+        <v>278198</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>10</v>
       </c>
       <c r="G10" s="2">
-        <v>3.55881</v>
+        <v>3.5588099999999998</v>
       </c>
       <c r="H10" s="2">
-        <v>3.920301</v>
+        <v>3.9203009999999998</v>
       </c>
       <c r="I10" s="2">
-        <v>0.6827</v>
+        <v>0.68269999999999997</v>
       </c>
       <c r="J10" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="4">
-        <v>40.780477924422</v>
+        <v>40.780477924422001</v>
       </c>
       <c r="B11" s="4">
-        <v>-73.9679390610308</v>
+        <v>-73.967939061030805</v>
       </c>
       <c r="C11" s="5">
-        <v>0.627920173079</v>
+        <v>0.62792017307900005</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E11" s="2">
-        <v>318233.0</v>
+        <v>318233</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>10</v>
       </c>
       <c r="G11" s="2">
-        <v>3.68891</v>
+        <v>3.6889099999999999</v>
       </c>
       <c r="H11" s="2">
         <v>2.049941</v>
       </c>
       <c r="I11" s="2">
-        <v>0.6827</v>
+        <v>0.68269999999999997</v>
       </c>
       <c r="J11" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
     </row>
-    <row r="13">
+    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
     </row>
-    <row r="14">
+    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="4"/>
       <c r="B14" s="3"/>
       <c r="C14" s="4"/>
     </row>
-    <row r="15">
+    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
     </row>
-    <row r="16">
+    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
     </row>
-    <row r="17">
+    <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
     </row>
-    <row r="18">
+    <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
     </row>
-    <row r="19">
+    <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
     </row>
-    <row r="20">
+    <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B20" s="4"/>
     </row>
-    <row r="21">
+    <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B21" s="4"/>
     </row>
-    <row r="22">
+    <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B22" s="4"/>
     </row>
-    <row r="23">
+    <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B23" s="4"/>
     </row>
-    <row r="24">
+    <row r="24" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B24" s="6"/>
     </row>
-    <row r="25">
+    <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B25" s="4"/>
     </row>
-    <row r="26">
+    <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B26" s="4"/>
     </row>
-    <row r="27">
+    <row r="27" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B27" s="4"/>
     </row>
-    <row r="41">
+    <row r="41" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B41" s="3"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:J41"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="19.13"/>
-    <col customWidth="1" min="2" max="2" width="18.5"/>
-    <col customWidth="1" min="4" max="4" width="9.75"/>
-    <col customWidth="1" min="7" max="7" width="17.88"/>
-    <col customWidth="1" min="8" max="8" width="17.13"/>
-    <col customWidth="1" min="9" max="9" width="28.75"/>
+    <col min="1" max="1" width="19.1640625" customWidth="1"/>
+    <col min="2" max="2" width="18.5" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" customWidth="1"/>
+    <col min="7" max="7" width="17.83203125" customWidth="1"/>
+    <col min="8" max="8" width="17.1640625" customWidth="1"/>
+    <col min="9" max="9" width="28.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1954,12 +1937,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="4">
-        <v>52.3719074577595</v>
+        <v>52.371907457759498</v>
       </c>
       <c r="B2" s="4">
-        <v>4.90526689003245</v>
+        <v>4.9052668900324496</v>
       </c>
       <c r="C2" s="6">
         <v>-1.39819542712897</v>
@@ -1968,71 +1951,71 @@
         <v>16</v>
       </c>
       <c r="E2" s="2">
-        <v>78.0</v>
+        <v>78</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>10</v>
       </c>
       <c r="G2" s="2">
-        <v>4.38821</v>
+        <v>4.3882099999999999</v>
       </c>
       <c r="H2" s="2">
-        <v>3.13234</v>
+        <v>3.1323400000000001</v>
       </c>
       <c r="I2" s="2">
-        <v>0.6827</v>
+        <v>0.68269999999999997</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="4">
-        <v>52.3714335866613</v>
+        <v>52.371433586661297</v>
       </c>
       <c r="B3" s="4">
-        <v>4.90409851493971</v>
+        <v>4.9040985149397098</v>
       </c>
       <c r="C3" s="4">
-        <v>-1.3085335092803</v>
+        <v>-1.3085335092803001</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E3" s="2">
-        <v>5781.0</v>
+        <v>5781</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>10</v>
       </c>
       <c r="G3" s="2">
-        <v>4.98133</v>
+        <v>4.9813299999999998</v>
       </c>
       <c r="H3" s="2">
-        <v>3.3291383</v>
+        <v>3.3291382999999999</v>
       </c>
       <c r="I3" s="2">
-        <v>0.6827</v>
+        <v>0.68269999999999997</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="4">
-        <v>52.3713044566592</v>
+        <v>52.371304456659203</v>
       </c>
       <c r="B4" s="4">
-        <v>4.9038118290386</v>
+        <v>4.9038118290385997</v>
       </c>
       <c r="C4" s="4">
-        <v>-0.0113110065885346</v>
+        <v>-1.13110065885346E-2</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E4" s="2">
-        <v>12785.0</v>
+        <v>12785</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>10</v>
@@ -2044,123 +2027,123 @@
         <v>3.39132933</v>
       </c>
       <c r="I4" s="2">
-        <v>0.6827</v>
+        <v>0.68269999999999997</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="4">
         <v>52.3711005552152</v>
       </c>
       <c r="B5" s="4">
-        <v>4.90411241094314</v>
+        <v>4.9041124109431404</v>
       </c>
       <c r="C5" s="4">
-        <v>-0.435420847930456</v>
+        <v>-0.43542084793045599</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E5" s="2">
-        <v>17636.0</v>
+        <v>17636</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="G5" s="2">
-        <v>4.596906</v>
+        <v>4.5969059999999997</v>
       </c>
       <c r="H5" s="2">
-        <v>3.585938</v>
+        <v>3.5859380000000001</v>
       </c>
       <c r="I5" s="2">
-        <v>0.6827</v>
+        <v>0.68269999999999997</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="4">
-        <v>52.3708876449937</v>
+        <v>52.370887644993701</v>
       </c>
       <c r="B6" s="4">
         <v>4.90427729624819</v>
       </c>
       <c r="C6" s="4">
-        <v>0.847999421928209</v>
+        <v>0.84799942192820899</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E6" s="2">
-        <v>23971.0</v>
+        <v>23971</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>10</v>
       </c>
       <c r="G6" s="2">
-        <v>4.89191</v>
+        <v>4.8919100000000002</v>
       </c>
       <c r="H6" s="2">
-        <v>3.981873</v>
+        <v>3.9818730000000002</v>
       </c>
       <c r="I6" s="2">
-        <v>0.6827</v>
+        <v>0.68269999999999997</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="4">
-        <v>52.3706592709929</v>
+        <v>52.370659270992903</v>
       </c>
       <c r="B7" s="4">
-        <v>4.90416842424938</v>
+        <v>4.9041684242493799</v>
       </c>
       <c r="C7" s="4">
-        <v>0.737749414369133</v>
+        <v>0.73774941436913299</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E7" s="2">
-        <v>29769.0</v>
+        <v>29769</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>10</v>
       </c>
       <c r="G7" s="2">
-        <v>4.8871812</v>
+        <v>4.8871811999999997</v>
       </c>
       <c r="H7" s="2">
-        <v>3.877172</v>
+        <v>3.8771719999999998</v>
       </c>
       <c r="I7" s="2">
-        <v>0.6827</v>
+        <v>0.68269999999999997</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="4">
-        <v>52.3703643529528</v>
+        <v>52.370364352952798</v>
       </c>
       <c r="B8" s="4">
-        <v>4.90450047223958</v>
+        <v>4.9045004722395804</v>
       </c>
       <c r="C8" s="4">
-        <v>0.666605798597992</v>
+        <v>0.66660579859799196</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E8" s="2">
-        <v>34521.0</v>
+        <v>34521</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>10</v>
@@ -2169,152 +2152,155 @@
         <v>4.721832</v>
       </c>
       <c r="H8" s="2">
-        <v>6.93301</v>
+        <v>6.9330100000000003</v>
       </c>
       <c r="I8" s="2">
-        <v>0.6827</v>
+        <v>0.68269999999999997</v>
       </c>
       <c r="J8" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="4">
-        <v>52.3705929507105</v>
+        <v>52.370592950710503</v>
       </c>
       <c r="B9" s="4">
         <v>4.90573079854871</v>
       </c>
       <c r="C9" s="4">
-        <v>0.692590480530808</v>
+        <v>0.69259048053080796</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E9" s="2">
-        <v>40818.0</v>
+        <v>40818</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>10</v>
       </c>
       <c r="G9" s="2">
-        <v>4.81812</v>
+        <v>4.8181200000000004</v>
       </c>
       <c r="H9" s="2">
         <v>3.93011</v>
       </c>
       <c r="I9" s="2">
-        <v>0.6827</v>
+        <v>0.68269999999999997</v>
       </c>
       <c r="J9" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
     </row>
-    <row r="12">
+    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
     </row>
-    <row r="13">
+    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
     </row>
-    <row r="14">
+    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="4"/>
       <c r="B14" s="3"/>
       <c r="C14" s="4"/>
     </row>
-    <row r="15">
+    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
     </row>
-    <row r="16">
+    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
     </row>
-    <row r="17">
+    <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
     </row>
-    <row r="18">
+    <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
     </row>
-    <row r="19">
+    <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
     </row>
-    <row r="20">
+    <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
     </row>
-    <row r="21">
+    <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
     </row>
-    <row r="22">
+    <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
     </row>
-    <row r="23">
+    <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
     </row>
-    <row r="24">
+    <row r="24" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="4"/>
       <c r="B24" s="6"/>
     </row>
-    <row r="25">
+    <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
     </row>
-    <row r="26">
+    <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
     </row>
-    <row r="27">
+    <row r="27" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B27" s="4"/>
     </row>
-    <row r="41">
+    <row r="41" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B41" s="3"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I37" sqref="I37"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="19.13"/>
-    <col customWidth="1" min="2" max="2" width="18.5"/>
-    <col customWidth="1" min="9" max="9" width="28.63"/>
+    <col min="1" max="1" width="19.1640625" customWidth="1"/>
+    <col min="2" max="2" width="18.5" customWidth="1"/>
+    <col min="9" max="9" width="28.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2346,140 +2332,140 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="4">
-        <v>51.5332793070309</v>
+        <v>51.533279307030902</v>
       </c>
       <c r="B2" s="4">
-        <v>-0.126299061684143</v>
+        <v>-0.12629906168414301</v>
       </c>
       <c r="C2" s="6">
-        <v>16.4669742326449</v>
+        <v>16.466974232644901</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E2" s="2">
-        <v>12918.0</v>
+        <v>12918</v>
       </c>
       <c r="F2" s="2">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="G2" s="2">
-        <v>21.2304</v>
+        <v>21.230399999999999</v>
       </c>
       <c r="H2" s="2">
-        <v>3.13902</v>
+        <v>3.1390199999999999</v>
       </c>
       <c r="I2" s="2">
-        <v>0.6827</v>
+        <v>0.68269999999999997</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="4">
-        <v>51.5333139586981</v>
+        <v>51.533313958698102</v>
       </c>
       <c r="B3" s="4">
-        <v>-0.126216115922224</v>
+        <v>-0.12621611592222401</v>
       </c>
       <c r="C3" s="4">
-        <v>16.7129042757665</v>
+        <v>16.712904275766501</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E3" s="2">
-        <v>133982.0</v>
+        <v>133982</v>
       </c>
       <c r="F3" s="2">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="G3" s="2">
-        <v>19.23299</v>
+        <v>19.232990000000001</v>
       </c>
       <c r="H3" s="2">
-        <v>4.930313</v>
+        <v>4.9303129999999999</v>
       </c>
       <c r="I3" s="2">
-        <v>0.6827</v>
+        <v>0.68269999999999997</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="4">
-        <v>51.5333115342771</v>
+        <v>51.533311534277097</v>
       </c>
       <c r="B4" s="4">
-        <v>-0.126159919379484</v>
+        <v>-0.12615991937948401</v>
       </c>
       <c r="C4" s="4">
-        <v>17.0438724202509</v>
+        <v>17.043872420250899</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E4" s="2">
-        <v>267813.0</v>
+        <v>267813</v>
       </c>
       <c r="F4" s="2">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="G4" s="2">
-        <v>18.2302031</v>
+        <v>18.230203100000001</v>
       </c>
       <c r="H4" s="2">
-        <v>4.39101</v>
+        <v>4.3910099999999996</v>
       </c>
       <c r="I4" s="2">
-        <v>0.6827</v>
+        <v>0.68269999999999997</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="4">
         <v>51.5333622516875</v>
       </c>
       <c r="B5" s="4">
-        <v>-0.126091690182172</v>
+        <v>-0.12609169018217201</v>
       </c>
       <c r="C5" s="4">
-        <v>17.9089128042998</v>
+        <v>17.908912804299799</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E5" s="2">
-        <v>401928.0</v>
+        <v>401928</v>
       </c>
       <c r="F5" s="2">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="G5" s="2">
         <v>17.420123</v>
       </c>
       <c r="H5" s="2">
-        <v>3.2931</v>
+        <v>3.2930999999999999</v>
       </c>
       <c r="I5" s="2">
-        <v>0.6827</v>
+        <v>0.68269999999999997</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="4">
-        <v>51.5334124621089</v>
+        <v>51.533412462108899</v>
       </c>
       <c r="B6" s="4">
-        <v>-0.126029362536468</v>
+        <v>-0.12602936253646799</v>
       </c>
       <c r="C6" s="4">
         <v>18.9072647148786</v>
@@ -2488,25 +2474,25 @@
         <v>12</v>
       </c>
       <c r="E6" s="2">
-        <v>530032.0</v>
+        <v>530032</v>
       </c>
       <c r="F6" s="2">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="G6" s="2">
-        <v>20.101393</v>
+        <v>20.101393000000002</v>
       </c>
       <c r="H6" s="2">
-        <v>4.239131</v>
+        <v>4.2391310000000004</v>
       </c>
       <c r="I6" s="2">
-        <v>0.6827</v>
+        <v>0.68269999999999997</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="4">
         <v>51.5333643352119</v>
       </c>
@@ -2520,30 +2506,30 @@
         <v>12</v>
       </c>
       <c r="E7" s="2">
-        <v>668321.0</v>
+        <v>668321</v>
       </c>
       <c r="F7" s="2">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="G7" s="2">
         <v>19.239023</v>
       </c>
       <c r="H7" s="2">
-        <v>3.931103</v>
+        <v>3.9311029999999998</v>
       </c>
       <c r="I7" s="2">
-        <v>0.6827</v>
+        <v>0.68269999999999997</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="4">
-        <v>51.533301888466</v>
+        <v>51.533301888465999</v>
       </c>
       <c r="B8" s="4">
-        <v>-0.125923225431633</v>
+        <v>-0.12592322543163301</v>
       </c>
       <c r="C8" s="4">
         <v>18.8110976622735</v>
@@ -2552,30 +2538,30 @@
         <v>12</v>
       </c>
       <c r="E8" s="2">
-        <v>798127.0</v>
+        <v>798127</v>
       </c>
       <c r="F8" s="2">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="G8" s="2">
         <v>19.2301942</v>
       </c>
       <c r="H8" s="2">
-        <v>3.29139193</v>
+        <v>3.2913919300000001</v>
       </c>
       <c r="I8" s="2">
-        <v>0.6827</v>
+        <v>0.68269999999999997</v>
       </c>
       <c r="J8" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="4">
-        <v>51.5331373721403</v>
+        <v>51.533137372140303</v>
       </c>
       <c r="B9" s="4">
-        <v>-0.126181551279945</v>
+        <v>-0.12618155127994499</v>
       </c>
       <c r="C9" s="4">
         <v>16.5417183521045</v>
@@ -2584,30 +2570,30 @@
         <v>14</v>
       </c>
       <c r="E9" s="2">
-        <v>9832.0</v>
+        <v>9832</v>
       </c>
       <c r="F9" s="2">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="G9" s="2">
-        <v>7.92391</v>
+        <v>7.9239100000000002</v>
       </c>
       <c r="H9" s="2">
-        <v>2.310931</v>
+        <v>2.3109310000000001</v>
       </c>
       <c r="I9" s="2">
-        <v>0.6827</v>
+        <v>0.68269999999999997</v>
       </c>
       <c r="J9" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="4">
-        <v>51.5331377164914</v>
+        <v>51.533137716491403</v>
       </c>
       <c r="B10" s="4">
-        <v>-0.126136502299829</v>
+        <v>-0.12613650229982901</v>
       </c>
       <c r="C10" s="4">
         <v>16.5766938347628</v>
@@ -2616,126 +2602,126 @@
         <v>14</v>
       </c>
       <c r="E10" s="2">
-        <v>98291.0</v>
+        <v>98291</v>
       </c>
       <c r="F10" s="2">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="G10" s="2">
-        <v>8.218313</v>
+        <v>8.2183130000000002</v>
       </c>
       <c r="H10" s="2">
-        <v>2.3283819</v>
+        <v>2.3283819000000001</v>
       </c>
       <c r="I10" s="2">
-        <v>0.6827</v>
+        <v>0.68269999999999997</v>
       </c>
       <c r="J10" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="4">
-        <v>51.5331882204422</v>
+        <v>51.533188220442199</v>
       </c>
       <c r="B11" s="4">
-        <v>-0.126112522362973</v>
+        <v>-0.12611252236297299</v>
       </c>
       <c r="C11" s="4">
-        <v>16.8028540476859</v>
+        <v>16.802854047685901</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E11" s="2">
-        <v>183273.0</v>
+        <v>183273</v>
       </c>
       <c r="F11" s="2">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="G11" s="2">
-        <v>7.3291</v>
+        <v>7.3291000000000004</v>
       </c>
       <c r="H11" s="2">
-        <v>3.8391293</v>
+        <v>3.8391293000000002</v>
       </c>
       <c r="I11" s="2">
-        <v>0.6827</v>
+        <v>0.68269999999999997</v>
       </c>
       <c r="J11" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="4">
-        <v>51.5332062692144</v>
+        <v>51.533206269214404</v>
       </c>
       <c r="B12" s="4">
-        <v>-0.126085420507433</v>
+        <v>-0.12608542050743299</v>
       </c>
       <c r="C12" s="4">
-        <v>17.0597738661109</v>
+        <v>17.059773866110898</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E12" s="2">
-        <v>278127.0</v>
+        <v>278127</v>
       </c>
       <c r="F12" s="2">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="G12" s="2">
-        <v>8.2382931</v>
+        <v>8.2382930999999999</v>
       </c>
       <c r="H12" s="2">
-        <v>3.2919392</v>
+        <v>3.2919391999999998</v>
       </c>
       <c r="I12" s="2">
-        <v>0.6827</v>
+        <v>0.68269999999999997</v>
       </c>
       <c r="J12" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="4">
-        <v>51.5332329769597</v>
+        <v>51.533232976959702</v>
       </c>
       <c r="B13" s="4">
         <v>-0.126045315693363</v>
       </c>
       <c r="C13" s="4">
-        <v>17.4283360357321</v>
+        <v>17.428336035732102</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E13" s="2">
-        <v>372819.0</v>
+        <v>372819</v>
       </c>
       <c r="F13" s="2">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="G13" s="2">
-        <v>7.1219301</v>
+        <v>7.1219301000000002</v>
       </c>
       <c r="H13" s="2">
-        <v>2.32494132</v>
+        <v>2.3249413200000002</v>
       </c>
       <c r="I13" s="2">
-        <v>0.6827</v>
+        <v>0.68269999999999997</v>
       </c>
       <c r="J13" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="4">
         <v>51.5332330953716</v>
       </c>
       <c r="B14" s="4">
-        <v>-0.125985470648224</v>
+        <v>-0.12598547064822399</v>
       </c>
       <c r="C14" s="4">
         <v>17.7493722549365</v>
@@ -2744,30 +2730,30 @@
         <v>14</v>
       </c>
       <c r="E14" s="2">
-        <v>469912.0</v>
+        <v>469912</v>
       </c>
       <c r="F14" s="2">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="G14" s="2">
-        <v>6.91481</v>
+        <v>6.9148100000000001</v>
       </c>
       <c r="H14" s="2">
         <v>3.9201302</v>
       </c>
       <c r="I14" s="2">
-        <v>0.6827</v>
+        <v>0.68269999999999997</v>
       </c>
       <c r="J14" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="4">
-        <v>51.5332718936936</v>
+        <v>51.533271893693602</v>
       </c>
       <c r="B15" s="4">
-        <v>-0.125918165282303</v>
+        <v>-0.12591816528230301</v>
       </c>
       <c r="C15" s="4">
         <v>18.6241685296628</v>
@@ -2776,148 +2762,147 @@
         <v>14</v>
       </c>
       <c r="E15" s="2">
-        <v>545913.0</v>
+        <v>545913</v>
       </c>
       <c r="F15" s="2">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="G15" s="2">
-        <v>6.93103</v>
+        <v>6.9310299999999998</v>
       </c>
       <c r="H15" s="2">
         <v>3.293931932</v>
       </c>
       <c r="I15" s="2">
-        <v>0.6827</v>
+        <v>0.68269999999999997</v>
       </c>
       <c r="J15" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="4">
-        <v>51.5333336558776</v>
+        <v>51.533333655877598</v>
       </c>
       <c r="B16" s="4">
-        <v>-0.125896857999116</v>
+        <v>-0.12589685799911601</v>
       </c>
       <c r="C16" s="4">
-        <v>19.3029835913135</v>
+        <v>19.302983591313499</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E16" s="2">
-        <v>645456.0</v>
+        <v>645456</v>
       </c>
       <c r="F16" s="2">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="G16" s="2">
-        <v>8.924902</v>
+        <v>8.9249019999999994</v>
       </c>
       <c r="H16" s="2">
         <v>2.3291013</v>
       </c>
       <c r="I16" s="2">
-        <v>0.6827</v>
+        <v>0.68269999999999997</v>
       </c>
       <c r="J16" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
     </row>
-    <row r="18">
+    <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
     </row>
-    <row r="19">
+    <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
     </row>
-    <row r="20">
+    <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
     </row>
-    <row r="21">
+    <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
     </row>
-    <row r="22">
+    <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
     </row>
-    <row r="23">
+    <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
     </row>
-    <row r="24">
+    <row r="24" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="4"/>
       <c r="B24" s="6"/>
     </row>
-    <row r="25">
+    <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
     </row>
-    <row r="26">
+    <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
     </row>
-    <row r="27">
+    <row r="27" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
     </row>
-    <row r="28">
+    <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="4"/>
     </row>
-    <row r="29">
+    <row r="29" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="4"/>
     </row>
-    <row r="30">
+    <row r="30" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="4"/>
     </row>
-    <row r="31">
+    <row r="31" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="4"/>
     </row>
-    <row r="32">
+    <row r="32" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="4"/>
     </row>
-    <row r="33">
+    <row r="33" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="4"/>
     </row>
-    <row r="34">
+    <row r="34" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="4"/>
     </row>
-    <row r="35">
+    <row r="35" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="4"/>
     </row>
-    <row r="41">
-      <c r="B41" s="3" t="s">
-        <v>18</v>
-      </c>
+    <row r="41" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B41" s="3"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2949,73 +2934,73 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2">
-        <v>37.8123987956971</v>
+        <v>37.812398795697099</v>
       </c>
       <c r="B2" s="2">
         <v>-122.362651703247</v>
       </c>
       <c r="C2" s="2">
-        <v>58.4398724664354</v>
+        <v>58.439872466435403</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="7">
+        <v>5589</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="8">
+        <v>50.165430000000001</v>
+      </c>
+      <c r="H2" s="9">
+        <v>15.234500000000001</v>
+      </c>
+      <c r="I2" s="2">
+        <v>0.68269999999999997</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="7">
-        <v>5589.0</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="8">
-        <v>50.16543</v>
-      </c>
-      <c r="H2" s="9">
-        <v>15.2345</v>
-      </c>
-      <c r="I2" s="2">
-        <v>0.6827</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3">
+    </row>
+    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2">
-        <v>37.8167527686732</v>
+        <v>37.816752768673197</v>
       </c>
       <c r="B3" s="2">
         <v>-122.355984717467</v>
       </c>
       <c r="C3" s="2">
-        <v>57.7555437701287</v>
+        <v>57.755543770128703</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="7">
+        <v>11401</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="8">
+        <v>25.365459999999999</v>
+      </c>
+      <c r="H3" s="9">
+        <v>6.4873799999999999</v>
+      </c>
+      <c r="I3" s="2">
+        <v>0.68269999999999997</v>
+      </c>
+      <c r="J3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="7">
-        <v>11401.0</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="8">
-        <v>25.36546</v>
-      </c>
-      <c r="H3" s="9">
-        <v>6.48738</v>
-      </c>
-      <c r="I3" s="2">
-        <v>0.6827</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4">
+    </row>
+    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2">
-        <v>37.8195572382245</v>
+        <v>37.819557238224498</v>
       </c>
       <c r="B4" s="2">
         <v>-122.346534098003</v>
@@ -3024,74 +3009,74 @@
         <v>57.7555735307944</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E4" s="7">
-        <v>16587.0</v>
+        <v>16587</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>10</v>
       </c>
       <c r="G4" s="8">
-        <v>20.44346</v>
+        <v>20.443460000000002</v>
       </c>
       <c r="H4" s="9">
         <v>6.48285</v>
       </c>
       <c r="I4" s="2">
-        <v>0.6827</v>
+        <v>0.68269999999999997</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2">
-        <v>37.8210495324005</v>
+        <v>37.821049532400501</v>
       </c>
       <c r="B5" s="2">
-        <v>-122.335691813646</v>
+        <v>-122.33569181364599</v>
       </c>
       <c r="C5" s="2">
-        <v>58.7539261981981</v>
+        <v>58.753926198198101</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E5" s="7">
-        <v>22478.0</v>
+        <v>22478</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="G5" s="8">
-        <v>20.18783</v>
+        <v>20.187830000000002</v>
       </c>
       <c r="H5" s="9">
         <v>6.21373</v>
       </c>
       <c r="I5" s="2">
-        <v>0.6827</v>
+        <v>0.68269999999999997</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2">
-        <v>37.8221633068431</v>
+        <v>37.822163306843102</v>
       </c>
       <c r="B6" s="2">
         <v>-122.323728033097</v>
       </c>
       <c r="C6" s="2">
-        <v>38.9154865846787</v>
+        <v>38.915486584678703</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E6" s="7">
-        <v>27731.0</v>
+        <v>27731</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>10</v>
@@ -3100,30 +3085,30 @@
         <v>15.1235</v>
       </c>
       <c r="H6" s="9">
-        <v>5.23723</v>
+        <v>5.2372300000000003</v>
       </c>
       <c r="I6" s="2">
-        <v>0.6827</v>
+        <v>0.68269999999999997</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2">
-        <v>37.8242236853699</v>
+        <v>37.824223685369901</v>
       </c>
       <c r="B7" s="2">
         <v>-122.31002242906</v>
       </c>
       <c r="C7" s="2">
-        <v>30.9105833708903</v>
+        <v>30.910583370890301</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E7" s="7">
-        <v>33435.0</v>
+        <v>33435</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>10</v>
@@ -3132,30 +3117,30 @@
         <v>14.27848</v>
       </c>
       <c r="H7" s="9">
-        <v>5.98438</v>
+        <v>5.9843799999999998</v>
       </c>
       <c r="I7" s="2">
-        <v>0.6827</v>
+        <v>0.68269999999999997</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2">
-        <v>37.8244999081891</v>
+        <v>37.824499908189097</v>
       </c>
       <c r="B8" s="2">
-        <v>-122.304915136127</v>
+        <v>-122.30491513612699</v>
       </c>
       <c r="C8" s="2">
-        <v>30.0738408098951</v>
+        <v>30.073840809895099</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E8" s="7">
-        <v>38750.0</v>
+        <v>38750</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>10</v>
@@ -3164,48 +3149,48 @@
         <v>16.123932</v>
       </c>
       <c r="H8" s="9">
-        <v>4.48284</v>
+        <v>4.4828400000000004</v>
       </c>
       <c r="I8" s="2">
-        <v>0.6827</v>
+        <v>0.68269999999999997</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2">
-        <v>37.8225366630228</v>
+        <v>37.822536663022802</v>
       </c>
       <c r="B9" s="2">
         <v>-122.300064053447</v>
       </c>
       <c r="C9" s="2">
-        <v>30.2838851006999</v>
+        <v>30.283885100699901</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E9" s="7">
-        <v>44006.0</v>
+        <v>44006</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>10</v>
       </c>
       <c r="G9" s="8">
-        <v>13.12478</v>
+        <v>13.124779999999999</v>
       </c>
       <c r="H9" s="9">
         <v>4.58394893</v>
       </c>
       <c r="I9" s="2">
-        <v>0.6827</v>
+        <v>0.68269999999999997</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2">
         <v>37.8201992000198</v>
       </c>
@@ -3213,13 +3198,13 @@
         <v>-122.296745932702</v>
       </c>
       <c r="C10" s="2">
-        <v>25.6659089131012</v>
+        <v>25.665908913101202</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E10" s="7">
-        <v>49284.0</v>
+        <v>49284</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>10</v>
@@ -3228,62 +3213,62 @@
         <v>14.12327</v>
       </c>
       <c r="H10" s="9">
-        <v>4.233823</v>
+        <v>4.2338230000000001</v>
       </c>
       <c r="I10" s="2">
-        <v>0.6827</v>
+        <v>0.68269999999999997</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2">
-        <v>37.8185141722501</v>
+        <v>37.818514172250097</v>
       </c>
       <c r="B11" s="2">
-        <v>-122.296834465024</v>
+        <v>-122.29683446502401</v>
       </c>
       <c r="C11" s="2">
         <v>24.5408154582436</v>
       </c>
       <c r="D11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="7">
+        <v>55117</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="8">
+        <v>14.128729999999999</v>
+      </c>
+      <c r="H11" s="9">
+        <v>4.2389229999999998</v>
+      </c>
+      <c r="I11" s="2">
+        <v>0.68269999999999997</v>
+      </c>
+      <c r="J11" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E11" s="7">
-        <v>55117.0</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G11" s="8">
-        <v>14.12873</v>
-      </c>
-      <c r="H11" s="9">
-        <v>4.238923</v>
-      </c>
-      <c r="I11" s="2">
-        <v>0.6827</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12">
+    </row>
+    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="2">
-        <v>37.8158233196927</v>
+        <v>37.815823319692697</v>
       </c>
       <c r="B12" s="2">
-        <v>-122.299586528561</v>
+        <v>-122.29958652856099</v>
       </c>
       <c r="C12" s="2">
-        <v>23.6659457448869</v>
+        <v>23.665945744886901</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E12" s="7">
-        <v>60971.0</v>
+        <v>60971</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>10</v>
@@ -3292,30 +3277,30 @@
         <v>14.8582</v>
       </c>
       <c r="H12" s="9">
-        <v>4.5893843</v>
+        <v>4.5893842999999999</v>
       </c>
       <c r="I12" s="2">
-        <v>0.6827</v>
+        <v>0.68269999999999997</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="2">
-        <v>37.8123082985971</v>
+        <v>37.812308298597102</v>
       </c>
       <c r="B13" s="2">
         <v>-122.303616521663</v>
       </c>
       <c r="C13" s="2">
-        <v>18.4833524686165</v>
+        <v>18.483352468616498</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E13" s="7">
-        <v>66118.0</v>
+        <v>66118</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>10</v>
@@ -3324,30 +3309,30 @@
         <v>12.40583</v>
       </c>
       <c r="H13" s="9">
-        <v>4.5986485</v>
+        <v>4.5986485000000004</v>
       </c>
       <c r="I13" s="2">
-        <v>0.6827</v>
+        <v>0.68269999999999997</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="2">
-        <v>37.8093552085929</v>
+        <v>37.809355208592898</v>
       </c>
       <c r="B14" s="2">
         <v>-122.304921845823</v>
       </c>
       <c r="C14" s="2">
-        <v>16.7388519220489</v>
+        <v>16.738851922048902</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E14" s="7">
-        <v>71481.0</v>
+        <v>71481</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>10</v>
@@ -3356,80 +3341,80 @@
         <v>15.28485</v>
       </c>
       <c r="H14" s="9">
-        <v>4.5983483</v>
+        <v>4.5983482999999996</v>
       </c>
       <c r="I14" s="2">
-        <v>0.6827</v>
+        <v>0.68269999999999997</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="2">
-        <v>37.8052802626972</v>
+        <v>37.805280262697202</v>
       </c>
       <c r="B15" s="2">
-        <v>-122.303897155045</v>
+        <v>-122.30389715504499</v>
       </c>
       <c r="C15" s="2">
         <v>15.5608413780335</v>
       </c>
       <c r="D15" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="7">
+        <v>76894</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15" s="8">
+        <v>12.482839999999999</v>
+      </c>
+      <c r="H15" s="9">
+        <v>4.4394340000000003</v>
+      </c>
+      <c r="I15" s="2">
+        <v>0.68269999999999997</v>
+      </c>
+      <c r="J15" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E15" s="7">
-        <v>76894.0</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G15" s="8">
-        <v>12.48284</v>
-      </c>
-      <c r="H15" s="9">
-        <v>4.439434</v>
-      </c>
-      <c r="I15" s="2">
-        <v>0.6827</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16">
+    </row>
+    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="2">
-        <v>37.8027797915371</v>
+        <v>37.802779791537098</v>
       </c>
       <c r="B16" s="2">
-        <v>-122.300790518126</v>
+        <v>-122.30079051812601</v>
       </c>
       <c r="C16" s="2">
         <v>13.571063227003</v>
       </c>
       <c r="D16" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" s="7">
+        <v>82145</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" s="8">
+        <v>10.284840000000001</v>
+      </c>
+      <c r="H16" s="9">
+        <v>4.7979500000000002</v>
+      </c>
+      <c r="I16" s="2">
+        <v>0.68269999999999997</v>
+      </c>
+      <c r="J16" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E16" s="7">
-        <v>82145.0</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G16" s="8">
-        <v>10.28484</v>
-      </c>
-      <c r="H16" s="9">
-        <v>4.79795</v>
-      </c>
-      <c r="I16" s="2">
-        <v>0.6827</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17">
+    </row>
+    <row r="17" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="2">
         <v>37.8017762513349</v>
       </c>
@@ -3437,45 +3422,45 @@
         <v>-122.29635830094</v>
       </c>
       <c r="C17" s="2">
-        <v>12.7451390043039</v>
+        <v>12.745139004303899</v>
       </c>
       <c r="D17" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" s="7">
+        <v>87595</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" s="8">
+        <v>10.273720000000001</v>
+      </c>
+      <c r="H17" s="9">
+        <v>5.2388399999999997</v>
+      </c>
+      <c r="I17" s="2">
+        <v>0.68269999999999997</v>
+      </c>
+      <c r="J17" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E17" s="7">
-        <v>87595.0</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G17" s="8">
-        <v>10.27372</v>
-      </c>
-      <c r="H17" s="9">
-        <v>5.23884</v>
-      </c>
-      <c r="I17" s="2">
-        <v>0.6827</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18">
+    </row>
+    <row r="18" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="2">
-        <v>37.8021696793913</v>
+        <v>37.802169679391298</v>
       </c>
       <c r="B18" s="2">
-        <v>-122.29236544818</v>
+        <v>-122.29236544818001</v>
       </c>
       <c r="C18" s="2">
-        <v>8.6657023475567</v>
+        <v>8.6657023475566994</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E18" s="7">
-        <v>93277.0</v>
+        <v>93277</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>10</v>
@@ -3484,48 +3469,48 @@
         <v>11.1958</v>
       </c>
       <c r="H18" s="9">
-        <v>5.472732</v>
+        <v>5.4727319999999997</v>
       </c>
       <c r="I18" s="2">
-        <v>0.6827</v>
+        <v>0.68269999999999997</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="2">
-        <v>37.8032280199733</v>
+        <v>37.803228019973297</v>
       </c>
       <c r="B19" s="2">
         <v>-122.291109432583</v>
       </c>
       <c r="C19" s="2">
-        <v>6.163646818183</v>
+        <v>6.1636468181830004</v>
       </c>
       <c r="D19" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E19" s="7">
+        <v>98692</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19" s="8">
+        <v>11.846220000000001</v>
+      </c>
+      <c r="H19" s="2">
+        <v>6.4728399999999997</v>
+      </c>
+      <c r="I19" s="2">
+        <v>0.68269999999999997</v>
+      </c>
+      <c r="J19" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E19" s="7">
-        <v>98692.0</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G19" s="8">
-        <v>11.84622</v>
-      </c>
-      <c r="H19" s="2">
-        <v>6.47284</v>
-      </c>
-      <c r="I19" s="2">
-        <v>0.6827</v>
-      </c>
-      <c r="J19" s="2" t="s">
-        <v>20</v>
-      </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>